<commit_message>
added hint messages to print in terminal.
</commit_message>
<xml_diff>
--- a/Managers.xlsx
+++ b/Managers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9163EC98-0B3B-4A1B-B3E2-00063E0D997A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E9AAC7-0903-44A6-988F-D766765496D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="888" yWindow="876" windowWidth="20076" windowHeight="11484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Manager Name</t>
   </si>
@@ -34,74 +34,47 @@
     <t>Set</t>
   </si>
   <si>
-    <t>Cyril Ellison</t>
-  </si>
-  <si>
-    <t>Edwena Wyman</t>
-  </si>
-  <si>
-    <t>Helen Fairchild</t>
-  </si>
-  <si>
-    <t>Kyro Horton</t>
-  </si>
-  <si>
-    <t>Jonette Lewis</t>
-  </si>
-  <si>
-    <t>Sylvan Aylmer</t>
-  </si>
-  <si>
-    <t>Marleen Garfield</t>
-  </si>
-  <si>
-    <t>Tanzi Seymour</t>
-  </si>
-  <si>
-    <t>Hayley Leonardson</t>
-  </si>
-  <si>
-    <t>Olive Jeffers</t>
-  </si>
-  <si>
-    <t>Chris Garrard</t>
-  </si>
-  <si>
-    <t>Derryl Harvey</t>
-  </si>
-  <si>
-    <t>Beryl Bass</t>
-  </si>
-  <si>
-    <t>Abbi Daniels</t>
-  </si>
-  <si>
-    <t>Jane Bone</t>
-  </si>
-  <si>
-    <t>Tucker Russel</t>
-  </si>
-  <si>
-    <t>Racheal Haley</t>
-  </si>
-  <si>
-    <t>Bryanne Franklin</t>
-  </si>
-  <si>
-    <t>Kimberley Romilly</t>
-  </si>
-  <si>
-    <t>Carolina Paxton</t>
-  </si>
-  <si>
     <t>Morning</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Tamar Khardziani</t>
+  </si>
+  <si>
+    <t>tkhardziani@evolution.com</t>
+  </si>
+  <si>
+    <t>Giorgi Gelovani</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>ggelovani@evolution.com</t>
+  </si>
+  <si>
+    <t>Anastasia Ioseiani</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>aioseliani@evolution.com</t>
+  </si>
+  <si>
+    <t>Nodar Gelovani</t>
+  </si>
+  <si>
+    <t>ngelovani@evolution.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +86,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,14 +116,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,19 +405,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,230 +428,75 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C21" xr:uid="{6153E5AE-A04E-4B17-84C8-66511227889C}"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1BC93F6B-3DEA-4D2A-BD06-54ADF3116F66}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{DEE45D3F-74C4-4274-9D50-2A48445B21B1}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{A20D248E-1C85-452B-BF4A-2F0A3BF39261}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{E56839AD-B952-485D-83E6-4621274C5258}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>